<commit_message>
version of the builder that builds the DOE template
</commit_message>
<xml_diff>
--- a/regolith/templates/coa_template_doe.xlsx
+++ b/regolith/templates/coa_template_doe.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gail/Desktop/Work/DoE Solar Fuels Hub Proposal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\dev\regolith\regolith\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E55920B1-CC34-7D4A-A9CC-ED9596B84DE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="2560" windowWidth="22840" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Collaborator Template" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Collaborator Template'!$6:$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Example!$6:$7</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Name of Lead Organization:</t>
   </si>
@@ -132,16 +131,13 @@
     <t>Alice</t>
   </si>
   <si>
-    <t>Massachusetts Institute of Technology</t>
-  </si>
-  <si>
-    <t>Roman, Yuriy</t>
+    <t>tbd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -532,21 +528,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="22.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="45.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -555,38 +551,38 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="str">
         <f>"Collaborator Table - "&amp;C1&amp;" ("&amp;C2&amp;")"</f>
-        <v>Collaborator Table - Massachusetts Institute of Technology (Roman, Yuriy)</v>
+        <v>Collaborator Table - tbd (tbd)</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -597,497 +593,497 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -1114,17 +1110,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="112.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="290.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="290.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -1136,7 +1132,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1144,13 +1140,13 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="22.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="44.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1159,7 +1155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1168,7 +1164,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1177,7 +1173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1186,7 +1182,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="str">
         <f>"Collaborator Table - "&amp;C1&amp;" ("&amp;C2&amp;")"</f>
         <v>Collaborator Table - University of XYZ (Jones, Jane)</v>
@@ -1194,7 +1190,7 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1205,7 +1201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1216,7 +1212,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1227,7 +1223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>

</xml_diff>